<commit_message>
Added test cases and makefile
</commit_message>
<xml_diff>
--- a/fileapp/uploads/files/2021_11_10_Phobs_download_boekingen_JV.xlsx
+++ b/fileapp/uploads/files/2021_11_10_Phobs_download_boekingen_JV.xlsx
@@ -11609,10 +11609,10 @@
   <dimension ref="A1:AA501"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.14"/>
@@ -11626,7 +11626,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="13.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="36.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="12.71"/>
@@ -11806,7 +11806,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>11439948</v>
       </c>
@@ -11887,7 +11887,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>11437630</v>
       </c>

</xml_diff>